<commit_message>
Atualizando modelo de importação da escala e testes referentes a importação da escala.
</commit_message>
<xml_diff>
--- a/apis/src/main/resources/samples/modelo_importacao_escala.xlsx
+++ b/apis/src/main/resources/samples/modelo_importacao_escala.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="99">
   <si>
     <t xml:space="preserve">Data de Criação</t>
   </si>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">Folga</t>
   </si>
   <si>
-    <t xml:space="preserve">REG874</t>
+    <t xml:space="preserve">REG00001</t>
   </si>
   <si>
     <t xml:space="preserve">CARLOS</t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">Tenente</t>
   </si>
   <si>
-    <t xml:space="preserve">REG532</t>
+    <t xml:space="preserve">REG00002</t>
   </si>
   <si>
     <t xml:space="preserve">ANA</t>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">Sargento</t>
   </si>
   <si>
-    <t xml:space="preserve">REG764</t>
+    <t xml:space="preserve">REG00017</t>
   </si>
   <si>
     <t xml:space="preserve">ALICE</t>
@@ -188,7 +188,7 @@
     <t xml:space="preserve">Cabo</t>
   </si>
   <si>
-    <t xml:space="preserve">REG294</t>
+    <t xml:space="preserve">REG00022</t>
   </si>
   <si>
     <t xml:space="preserve">JOANA</t>
@@ -197,124 +197,124 @@
     <t xml:space="preserve">Soldado</t>
   </si>
   <si>
-    <t xml:space="preserve">REG561</t>
+    <t xml:space="preserve">REG00023</t>
   </si>
   <si>
     <t xml:space="preserve">GUSTAVO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG687</t>
+    <t xml:space="preserve">REG00003</t>
   </si>
   <si>
     <t xml:space="preserve">JOÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG193</t>
+    <t xml:space="preserve">REG00015</t>
   </si>
   <si>
     <t xml:space="preserve">JULIANA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG405</t>
+    <t xml:space="preserve">REG00016</t>
   </si>
   <si>
     <t xml:space="preserve">MARCOS</t>
   </si>
   <si>
-    <t xml:space="preserve">REG713</t>
+    <t xml:space="preserve">REG00020</t>
   </si>
   <si>
     <t xml:space="preserve">HENRIQUE</t>
   </si>
   <si>
-    <t xml:space="preserve">REG418</t>
+    <t xml:space="preserve">REG00021</t>
   </si>
   <si>
     <t xml:space="preserve">PEDRO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG920</t>
+    <t xml:space="preserve">REG00004</t>
   </si>
   <si>
     <t xml:space="preserve">PAULO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG273</t>
+    <t xml:space="preserve">REG00008</t>
   </si>
   <si>
     <t xml:space="preserve">ROBERTO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG582</t>
+    <t xml:space="preserve">REG00014</t>
   </si>
   <si>
     <t xml:space="preserve">LUCAS</t>
   </si>
   <si>
-    <t xml:space="preserve">REG328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REG412</t>
+    <t xml:space="preserve">REG00018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REG00019</t>
   </si>
   <si>
     <t xml:space="preserve">SOFIA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG385</t>
+    <t xml:space="preserve">REG00005</t>
   </si>
   <si>
     <t xml:space="preserve">MARIANA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG835</t>
+    <t xml:space="preserve">REG00011</t>
   </si>
   <si>
     <t xml:space="preserve">LETÍCIA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG104</t>
+    <t xml:space="preserve">REG00009</t>
   </si>
   <si>
     <t xml:space="preserve">FERNANDA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG672</t>
+    <t xml:space="preserve">REG00010</t>
   </si>
   <si>
     <t xml:space="preserve">ANDRÉ</t>
   </si>
   <si>
-    <t xml:space="preserve">REG329</t>
+    <t xml:space="preserve">REG00012</t>
   </si>
   <si>
     <t xml:space="preserve">BRUNO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG741</t>
+    <t xml:space="preserve">REG00006</t>
   </si>
   <si>
     <t xml:space="preserve">RAFAEL</t>
   </si>
   <si>
-    <t xml:space="preserve">REG450</t>
+    <t xml:space="preserve">REG00013</t>
   </si>
   <si>
     <t xml:space="preserve">CARLA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG829</t>
+    <t xml:space="preserve">REG00007</t>
   </si>
   <si>
     <t xml:space="preserve">CAMILA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG873</t>
+    <t xml:space="preserve">REG00024</t>
   </si>
   <si>
     <t xml:space="preserve">ADRIANA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG690</t>
+    <t xml:space="preserve">REG00025</t>
   </si>
   <si>
     <t xml:space="preserve">FELIPE</t>
@@ -577,10 +577,10 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.07"/>
@@ -620,28 +620,28 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>45981</v>
+        <v>46033</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45536</v>
+        <v>46023</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45537</v>
+        <v>46024</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45538</v>
+        <v>46025</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45539</v>
+        <v>46026</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45540</v>
+        <v>46027</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45541</v>
+        <v>46028</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45542</v>
+        <v>46029</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,25 +827,25 @@
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="n">
-        <v>45543</v>
+        <v>46030</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45544</v>
+        <v>46031</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>45545</v>
+        <v>46032</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>45546</v>
+        <v>46033</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45547</v>
+        <v>46034</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>45548</v>
+        <v>46035</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45549</v>
+        <v>46036</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +859,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
@@ -911,7 +911,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>23</v>
@@ -937,7 +937,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>22</v>
@@ -1031,25 +1031,25 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="n">
-        <v>45550</v>
+        <v>46037</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45551</v>
+        <v>46038</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>45552</v>
+        <v>46039</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>45553</v>
+        <v>46040</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>45554</v>
+        <v>46041</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>45555</v>
+        <v>46042</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>45556</v>
+        <v>46043</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,13 +1069,13 @@
         <v>10</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,7 +1101,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,19 +1115,19 @@
         <v>21</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,25 +1235,25 @@
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="2" t="n">
-        <v>45557</v>
+        <v>46044</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45558</v>
+        <v>46045</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45559</v>
+        <v>46046</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>45560</v>
+        <v>46047</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>45561</v>
+        <v>46048</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>45562</v>
+        <v>46049</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>45563</v>
+        <v>46050</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,13 +1261,13 @@
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>21</v>
@@ -1276,10 +1276,10 @@
         <v>21</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,25 +1287,25 @@
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,7 +1313,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>33</v>
@@ -1342,10 +1342,10 @@
         <v>22</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>22</v>
@@ -1368,7 +1368,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>29</v>
@@ -1397,7 +1397,7 @@
         <v>29</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>26</v>
@@ -1420,8 +1420,12 @@
       <c r="C33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1429,13 +1433,17 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="n">
-        <v>45564</v>
+        <v>46051</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+        <v>46052</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>46053</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>46054</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -1445,16 +1453,16 @@
         <v>8</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>22</v>
@@ -1471,16 +1479,16 @@
         <v>13</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>22</v>
@@ -1497,16 +1505,16 @@
         <v>17</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>22</v>
@@ -1523,16 +1531,16 @@
         <v>17</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>22</v>
@@ -1555,10 +1563,10 @@
         <v>27</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>22</v>
@@ -1581,10 +1589,10 @@
         <v>30</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>22</v>
@@ -1612,16 +1620,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G157"/>
+  <dimension ref="A1:G172"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.05"/>
@@ -1654,7 +1662,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>45536</v>
+        <v>46023</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>46</v>
@@ -1672,12 +1680,12 @@
         <v>8</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
-        <v>45536</v>
+        <v>46023</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>49</v>
@@ -1700,7 +1708,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
-        <v>45536</v>
+        <v>46023</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
@@ -1712,7 +1720,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -1723,7 +1731,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>45536</v>
+        <v>46023</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>55</v>
@@ -1735,7 +1743,7 @@
         <v>57</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>24</v>
@@ -1746,7 +1754,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
-        <v>45536</v>
+        <v>46023</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>58</v>
@@ -1758,7 +1766,7 @@
         <v>57</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>32</v>
@@ -1769,7 +1777,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
-        <v>45537</v>
+        <v>46024</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>46</v>
@@ -1787,12 +1795,12 @@
         <v>8</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>45537</v>
+        <v>46024</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>49</v>
@@ -1815,7 +1823,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <v>45537</v>
+        <v>46024</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>52</v>
@@ -1827,7 +1835,7 @@
         <v>54</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>17</v>
@@ -1838,7 +1846,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
-        <v>45537</v>
+        <v>46024</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>58</v>
@@ -1850,7 +1858,7 @@
         <v>57</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>24</v>
@@ -1861,7 +1869,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
-        <v>45537</v>
+        <v>46024</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>55</v>
@@ -1873,7 +1881,7 @@
         <v>57</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>32</v>
@@ -1884,7 +1892,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
-        <v>45538</v>
+        <v>46025</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>60</v>
@@ -1902,12 +1910,12 @@
         <v>8</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
-        <v>45538</v>
+        <v>46025</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>60</v>
@@ -1930,7 +1938,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
-        <v>45538</v>
+        <v>46025</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>62</v>
@@ -1942,7 +1950,7 @@
         <v>54</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
@@ -1953,7 +1961,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
-        <v>45538</v>
+        <v>46025</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>64</v>
@@ -1965,7 +1973,7 @@
         <v>54</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>17</v>
@@ -1976,7 +1984,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
-        <v>45538</v>
+        <v>46025</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>66</v>
@@ -1988,7 +1996,7 @@
         <v>57</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>24</v>
@@ -1999,7 +2007,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
-        <v>45538</v>
+        <v>46025</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>68</v>
@@ -2011,7 +2019,7 @@
         <v>57</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>32</v>
@@ -2022,7 +2030,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
-        <v>45539</v>
+        <v>46026</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>60</v>
@@ -2040,12 +2048,12 @@
         <v>8</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
-        <v>45539</v>
+        <v>46026</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>60</v>
@@ -2068,7 +2076,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
-        <v>45539</v>
+        <v>46026</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>62</v>
@@ -2080,7 +2088,7 @@
         <v>54</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>17</v>
@@ -2091,7 +2099,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
-        <v>45539</v>
+        <v>46026</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>64</v>
@@ -2103,7 +2111,7 @@
         <v>54</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>17</v>
@@ -2114,7 +2122,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
-        <v>45539</v>
+        <v>46026</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>68</v>
@@ -2126,7 +2134,7 @@
         <v>57</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>24</v>
@@ -2137,7 +2145,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
-        <v>45539</v>
+        <v>46026</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>66</v>
@@ -2149,7 +2157,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>32</v>
@@ -2160,7 +2168,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
-        <v>45540</v>
+        <v>46027</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>70</v>
@@ -2178,12 +2186,12 @@
         <v>8</v>
       </c>
       <c r="G24" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
-        <v>45540</v>
+        <v>46027</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>72</v>
@@ -2195,7 +2203,7 @@
         <v>54</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>13</v>
@@ -2206,7 +2214,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
-        <v>45540</v>
+        <v>46027</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>74</v>
@@ -2218,7 +2226,7 @@
         <v>54</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>17</v>
@@ -2229,7 +2237,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
-        <v>45540</v>
+        <v>46027</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>76</v>
@@ -2241,7 +2249,7 @@
         <v>57</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>24</v>
@@ -2252,7 +2260,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
-        <v>45540</v>
+        <v>46027</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>77</v>
@@ -2264,7 +2272,7 @@
         <v>57</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>32</v>
@@ -2275,7 +2283,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
-        <v>45541</v>
+        <v>46028</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>70</v>
@@ -2293,12 +2301,12 @@
         <v>8</v>
       </c>
       <c r="G29" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
-        <v>45541</v>
+        <v>46028</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>72</v>
@@ -2310,7 +2318,7 @@
         <v>54</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>13</v>
@@ -2321,7 +2329,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
-        <v>45541</v>
+        <v>46028</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>74</v>
@@ -2333,7 +2341,7 @@
         <v>54</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>17</v>
@@ -2344,7 +2352,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
-        <v>45541</v>
+        <v>46028</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>77</v>
@@ -2356,7 +2364,7 @@
         <v>57</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>24</v>
@@ -2367,7 +2375,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="n">
-        <v>45541</v>
+        <v>46028</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>76</v>
@@ -2379,7 +2387,7 @@
         <v>57</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>32</v>
@@ -2390,7 +2398,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
-        <v>45542</v>
+        <v>46029</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>79</v>
@@ -2408,12 +2416,12 @@
         <v>8</v>
       </c>
       <c r="G34" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="n">
-        <v>45542</v>
+        <v>46029</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>81</v>
@@ -2425,18 +2433,18 @@
         <v>54</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G35" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="n">
-        <v>45542</v>
+        <v>46029</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>83</v>
@@ -2448,7 +2456,7 @@
         <v>54</v>
       </c>
       <c r="E36" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>17</v>
@@ -2459,7 +2467,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="n">
-        <v>45542</v>
+        <v>46029</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>85</v>
@@ -2471,7 +2479,7 @@
         <v>54</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>24</v>
@@ -2482,7 +2490,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
-        <v>45542</v>
+        <v>46029</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>87</v>
@@ -2494,7 +2502,7 @@
         <v>54</v>
       </c>
       <c r="E38" s="3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>32</v>
@@ -2505,7 +2513,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="n">
-        <v>45543</v>
+        <v>46030</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>79</v>
@@ -2523,12 +2531,12 @@
         <v>8</v>
       </c>
       <c r="G39" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="n">
-        <v>45543</v>
+        <v>46030</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>81</v>
@@ -2540,18 +2548,18 @@
         <v>54</v>
       </c>
       <c r="E40" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="n">
-        <v>45543</v>
+        <v>46030</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>83</v>
@@ -2563,7 +2571,7 @@
         <v>54</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>17</v>
@@ -2574,7 +2582,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="n">
-        <v>45543</v>
+        <v>46030</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>87</v>
@@ -2586,7 +2594,7 @@
         <v>54</v>
       </c>
       <c r="E42" s="3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>24</v>
@@ -2597,7 +2605,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="n">
-        <v>45543</v>
+        <v>46030</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>85</v>
@@ -2609,7 +2617,7 @@
         <v>54</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>32</v>
@@ -2620,7 +2628,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="n">
-        <v>45544</v>
+        <v>46031</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>89</v>
@@ -2632,18 +2640,18 @@
         <v>54</v>
       </c>
       <c r="E44" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G44" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="n">
-        <v>45544</v>
+        <v>46031</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>91</v>
@@ -2655,7 +2663,7 @@
         <v>54</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>13</v>
@@ -2666,7 +2674,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="n">
-        <v>45544</v>
+        <v>46031</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>52</v>
@@ -2678,7 +2686,7 @@
         <v>54</v>
       </c>
       <c r="E46" s="3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>17</v>
@@ -2689,7 +2697,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="n">
-        <v>45544</v>
+        <v>46031</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>58</v>
@@ -2701,7 +2709,7 @@
         <v>57</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>24</v>
@@ -2712,7 +2720,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="n">
-        <v>45544</v>
+        <v>46031</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>93</v>
@@ -2724,7 +2732,7 @@
         <v>54</v>
       </c>
       <c r="E48" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>32</v>
@@ -2735,30 +2743,30 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="n">
-        <v>45545</v>
+        <v>46032</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G49" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="n">
-        <v>45545</v>
+        <v>46032</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>91</v>
@@ -2770,7 +2778,7 @@
         <v>54</v>
       </c>
       <c r="E50" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>13</v>
@@ -2781,19 +2789,19 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="n">
-        <v>45545</v>
+        <v>46032</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>17</v>
@@ -2804,22 +2812,22 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="n">
-        <v>45545</v>
+        <v>46032</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G52" s="3" t="n">
         <v>3</v>
@@ -2827,22 +2835,22 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="n">
-        <v>45545</v>
+        <v>46032</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G53" s="3" t="n">
         <v>3</v>
@@ -2850,91 +2858,91 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="n">
-        <v>45546</v>
+        <v>46032</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G54" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="n">
-        <v>45546</v>
+        <v>46033</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G55" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="n">
-        <v>45546</v>
+        <v>46033</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E56" s="3" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G56" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="n">
-        <v>45546</v>
+        <v>46033</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G57" s="3" t="n">
         <v>3</v>
@@ -2942,13 +2950,13 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="n">
-        <v>45546</v>
+        <v>46033</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>57</v>
@@ -2957,7 +2965,7 @@
         <v>27</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G58" s="3" t="n">
         <v>3</v>
@@ -2965,91 +2973,91 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="n">
-        <v>45547</v>
+        <v>46033</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G59" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="n">
-        <v>45547</v>
+        <v>46034</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G60" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="n">
-        <v>45547</v>
+        <v>46034</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G61" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="n">
-        <v>45547</v>
+        <v>46034</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E62" s="3" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G62" s="3" t="n">
         <v>3</v>
@@ -3057,22 +3065,22 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="n">
-        <v>45547</v>
+        <v>46034</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G63" s="3" t="n">
         <v>3</v>
@@ -3080,91 +3088,91 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="n">
-        <v>45548</v>
+        <v>46034</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E64" s="3" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G64" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="n">
-        <v>45548</v>
+        <v>46035</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G65" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="n">
-        <v>45548</v>
+        <v>46035</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G66" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="n">
-        <v>45548</v>
+        <v>46035</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G67" s="3" t="n">
         <v>3</v>
@@ -3172,13 +3180,13 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="n">
-        <v>45548</v>
+        <v>46035</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>57</v>
@@ -3187,7 +3195,7 @@
         <v>25</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G68" s="3" t="n">
         <v>3</v>
@@ -3195,91 +3203,91 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="n">
-        <v>45549</v>
+        <v>46035</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G69" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="n">
-        <v>45549</v>
+        <v>46036</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E70" s="3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G70" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="n">
-        <v>45549</v>
+        <v>46036</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G71" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="n">
-        <v>45549</v>
+        <v>46036</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E72" s="3" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G72" s="3" t="n">
         <v>3</v>
@@ -3287,22 +3295,22 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="n">
-        <v>45549</v>
+        <v>46036</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E73" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="G73" s="3" t="n">
         <v>3</v>
@@ -3310,30 +3318,30 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="n">
-        <v>45550</v>
+        <v>46036</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G74" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="n">
-        <v>45550</v>
+        <v>46037</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>49</v>
@@ -3348,44 +3356,44 @@
         <v>6</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G75" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="n">
-        <v>45550</v>
+        <v>46037</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E76" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="G76" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="n">
-        <v>45550</v>
+        <v>46037</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>54</v>
@@ -3402,22 +3410,22 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="n">
-        <v>45550</v>
+        <v>46037</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E78" s="3" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G78" s="3" t="n">
         <v>3</v>
@@ -3425,22 +3433,22 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="n">
-        <v>45550</v>
+        <v>46037</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E79" s="3" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G79" s="3" t="n">
         <v>3</v>
@@ -3448,30 +3456,30 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="n">
-        <v>45551</v>
+        <v>46037</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G80" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="n">
-        <v>45551</v>
+        <v>46038</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>49</v>
@@ -3486,44 +3494,44 @@
         <v>6</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G81" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="n">
-        <v>45551</v>
+        <v>46038</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E82" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="G82" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="n">
-        <v>45551</v>
+        <v>46038</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>54</v>
@@ -3540,22 +3548,22 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="n">
-        <v>45551</v>
+        <v>46038</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G84" s="3" t="n">
         <v>3</v>
@@ -3563,22 +3571,22 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="n">
-        <v>45551</v>
+        <v>46038</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G85" s="3" t="n">
         <v>3</v>
@@ -3586,30 +3594,30 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="n">
-        <v>45552</v>
+        <v>46038</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G86" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="n">
-        <v>45552</v>
+        <v>46039</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>60</v>
@@ -3624,44 +3632,44 @@
         <v>7</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G87" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="n">
-        <v>45552</v>
+        <v>46039</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E88" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G88" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="n">
-        <v>45552</v>
+        <v>46039</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>54</v>
@@ -3678,22 +3686,22 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="n">
-        <v>45552</v>
+        <v>46039</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G90" s="3" t="n">
         <v>3</v>
@@ -3701,22 +3709,22 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="n">
-        <v>45552</v>
+        <v>46039</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E91" s="3" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G91" s="3" t="n">
         <v>3</v>
@@ -3724,30 +3732,30 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="n">
-        <v>45553</v>
+        <v>46039</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G92" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="n">
-        <v>45553</v>
+        <v>46040</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>60</v>
@@ -3762,44 +3770,44 @@
         <v>7</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G93" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="n">
-        <v>45553</v>
+        <v>46040</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E94" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G94" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="n">
-        <v>45553</v>
+        <v>46040</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>54</v>
@@ -3816,22 +3824,22 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="n">
-        <v>45553</v>
+        <v>46040</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E96" s="3" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G96" s="3" t="n">
         <v>3</v>
@@ -3839,22 +3847,22 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="n">
-        <v>45553</v>
+        <v>46040</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G97" s="3" t="n">
         <v>3</v>
@@ -3862,91 +3870,91 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="n">
-        <v>45554</v>
+        <v>46040</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E98" s="3" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G98" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="n">
-        <v>45554</v>
+        <v>46041</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E99" s="3" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G99" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="n">
-        <v>45554</v>
+        <v>46041</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E100" s="3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G100" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="n">
-        <v>45554</v>
+        <v>46041</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E101" s="3" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G101" s="3" t="n">
         <v>3</v>
@@ -3954,13 +3962,13 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="n">
-        <v>45554</v>
+        <v>46041</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>57</v>
@@ -3969,7 +3977,7 @@
         <v>27</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G102" s="3" t="n">
         <v>3</v>
@@ -3977,91 +3985,91 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="n">
-        <v>45555</v>
+        <v>46041</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E103" s="3" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G103" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="n">
-        <v>45555</v>
+        <v>46042</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E104" s="3" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G104" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="n">
-        <v>45555</v>
+        <v>46042</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E105" s="3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G105" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="n">
-        <v>45555</v>
+        <v>46042</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E106" s="3" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G106" s="3" t="n">
         <v>3</v>
@@ -4069,22 +4077,22 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="n">
-        <v>45555</v>
+        <v>46042</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E107" s="3" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G107" s="3" t="n">
         <v>3</v>
@@ -4092,45 +4100,45 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="n">
-        <v>45556</v>
+        <v>46042</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E108" s="3" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G108" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="n">
-        <v>45556</v>
+        <v>46043</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E109" s="3" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G109" s="3" t="n">
         <v>3</v>
@@ -4138,45 +4146,45 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="n">
-        <v>45556</v>
+        <v>46043</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E110" s="3" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G110" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="n">
-        <v>45556</v>
+        <v>46043</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G111" s="3" t="n">
         <v>3</v>
@@ -4184,45 +4192,45 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="n">
-        <v>45557</v>
+        <v>46043</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E112" s="3" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G112" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="n">
-        <v>45557</v>
+        <v>46043</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E113" s="3" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G113" s="3" t="n">
         <v>3</v>
@@ -4230,22 +4238,22 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="n">
-        <v>45557</v>
+        <v>46044</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E114" s="3" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G114" s="3" t="n">
         <v>3</v>
@@ -4253,91 +4261,91 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="n">
-        <v>45557</v>
+        <v>46044</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E115" s="3" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="G115" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="n">
-        <v>45558</v>
+        <v>46044</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E116" s="3" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G116" s="3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="n">
-        <v>45558</v>
+        <v>46044</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E117" s="3" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G117" s="3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="n">
-        <v>45558</v>
+        <v>46044</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E118" s="3" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G118" s="3" t="n">
         <v>3</v>
@@ -4345,22 +4353,22 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="n">
-        <v>45558</v>
+        <v>46045</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G119" s="3" t="n">
         <v>3</v>
@@ -4368,45 +4376,45 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="n">
-        <v>45558</v>
+        <v>46045</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E120" s="3" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G120" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="n">
-        <v>45558</v>
+        <v>46045</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E121" s="3" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G121" s="3" t="n">
         <v>3</v>
@@ -4414,68 +4422,68 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="n">
-        <v>45559</v>
+        <v>46045</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E122" s="3" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G122" s="3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="n">
-        <v>45559</v>
+        <v>46045</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E123" s="3" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G123" s="3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="n">
-        <v>45559</v>
+        <v>46046</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E124" s="3" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G124" s="3" t="n">
         <v>3</v>
@@ -4483,13 +4491,13 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="n">
-        <v>45559</v>
+        <v>46046</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>54</v>
@@ -4498,30 +4506,30 @@
         <v>18</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G125" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="n">
-        <v>45559</v>
+        <v>46046</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E126" s="3" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G126" s="3" t="n">
         <v>3</v>
@@ -4529,22 +4537,22 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="n">
-        <v>45559</v>
+        <v>46046</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E127" s="3" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G127" s="3" t="n">
         <v>3</v>
@@ -4552,91 +4560,91 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="n">
-        <v>45560</v>
+        <v>46046</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E128" s="3" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G128" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="n">
-        <v>45560</v>
+        <v>46047</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E129" s="3" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G129" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="n">
-        <v>45560</v>
+        <v>46047</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E130" s="3" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G130" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="n">
-        <v>45560</v>
+        <v>46047</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E131" s="3" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G131" s="3" t="n">
         <v>3</v>
@@ -4644,22 +4652,22 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="n">
-        <v>45560</v>
+        <v>46047</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E132" s="3" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G132" s="3" t="n">
         <v>3</v>
@@ -4667,91 +4675,91 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="n">
-        <v>45561</v>
+        <v>46047</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E133" s="3" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G133" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="n">
-        <v>45561</v>
+        <v>46048</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E134" s="3" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G134" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="n">
-        <v>45561</v>
+        <v>46048</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E135" s="3" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G135" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="n">
-        <v>45561</v>
+        <v>46048</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E136" s="3" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G136" s="3" t="n">
         <v>3</v>
@@ -4759,22 +4767,22 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="n">
-        <v>45561</v>
+        <v>46048</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E137" s="3" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G137" s="3" t="n">
         <v>3</v>
@@ -4782,91 +4790,91 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="n">
-        <v>45562</v>
+        <v>46048</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E138" s="3" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G138" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="n">
-        <v>45562</v>
+        <v>46049</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G139" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="n">
-        <v>45562</v>
+        <v>46049</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E140" s="3" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G140" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="n">
-        <v>45562</v>
+        <v>46049</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E141" s="3" t="n">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G141" s="3" t="n">
         <v>3</v>
@@ -4874,13 +4882,13 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="n">
-        <v>45562</v>
+        <v>46049</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>57</v>
@@ -4889,7 +4897,7 @@
         <v>27</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G142" s="3" t="n">
         <v>3</v>
@@ -4897,91 +4905,91 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="n">
-        <v>45563</v>
+        <v>46049</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E143" s="3" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G143" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="5" t="n">
-        <v>45563</v>
+        <v>46050</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E144" s="3" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G144" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="5" t="n">
-        <v>45563</v>
+        <v>46050</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G145" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="n">
-        <v>45563</v>
+        <v>46050</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E146" s="3" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G146" s="3" t="n">
         <v>3</v>
@@ -4989,22 +4997,22 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="n">
-        <v>45563</v>
+        <v>46050</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G147" s="3" t="n">
         <v>3</v>
@@ -5012,91 +5020,91 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="n">
-        <v>45564</v>
+        <v>46050</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E148" s="3" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G148" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="n">
-        <v>45564</v>
+        <v>46051</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E149" s="3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G149" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="n">
-        <v>45564</v>
+        <v>46051</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E150" s="3" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G150" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="5" t="n">
-        <v>45564</v>
+        <v>46051</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G151" s="3" t="n">
         <v>3</v>
@@ -5104,22 +5112,22 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="n">
-        <v>45564</v>
+        <v>46051</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E152" s="3" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G152" s="3" t="n">
         <v>3</v>
@@ -5127,68 +5135,68 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="5" t="n">
-        <v>45565</v>
+        <v>46051</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G153" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="n">
-        <v>45565</v>
+        <v>46051</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E154" s="3" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G154" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="5" t="n">
-        <v>45565</v>
+        <v>46052</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E155" s="3" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G155" s="3" t="n">
         <v>3</v>
@@ -5196,47 +5204,392 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="n">
-        <v>45565</v>
+        <v>46052</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E156" s="3" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G156" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="5" t="n">
-        <v>45565</v>
+        <v>46052</v>
       </c>
       <c r="B157" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E157" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G157" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="5" t="n">
+        <v>46052</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E158" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G158" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="5" t="n">
+        <v>46052</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E159" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G159" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="5" t="n">
+        <v>46052</v>
+      </c>
+      <c r="B160" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C157" s="3" t="s">
+      <c r="C160" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D160" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E157" s="3" t="n">
+      <c r="E160" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G160" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="5" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E161" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G161" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="5" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E162" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G162" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="5" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E163" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G163" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="5" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E164" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G164" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="5" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E165" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F165" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F157" s="3" t="s">
+      <c r="G165" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="5" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E166" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F166" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G157" s="3" t="n">
+      <c r="G166" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="5" t="n">
+        <v>46054</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E167" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G167" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="5" t="n">
+        <v>46054</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E168" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G168" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="5" t="n">
+        <v>46054</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E169" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G169" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="5" t="n">
+        <v>46054</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E170" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G170" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="5" t="n">
+        <v>46054</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E171" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G171" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="5" t="n">
+        <v>46054</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E172" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G172" s="3" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>